<commit_message>
Allow null value on importer
</commit_message>
<xml_diff>
--- a/django_project/geosight/importer/tests/importers/_fixtures/excel_long_indicator_value (Multiple Value).xlsx
+++ b/django_project/geosight/importer/tests/importers/_fixtures/excel_long_indicator_value (Multiple Value).xlsx
@@ -16,15 +16,15 @@
   <definedNames/>
   <calcPr/>
   <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataSignature="AMtx7mi+UXBatFQzSAx8cjkAiPuZUmlApg=="/>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataChecksum="bmnISD6dnFMPociqsA5vDh98py0/G5yI1GEptyUpKng="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="20">
   <si>
     <t>geom_code</t>
   </si>
@@ -96,7 +96,7 @@
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -111,11 +111,6 @@
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -137,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -146,9 +141,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
@@ -157,12 +149,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="167" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
@@ -444,12 +430,12 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" ht="13.5" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -458,24 +444,24 @@
       <c r="C2" s="2">
         <v>4.5</v>
       </c>
-      <c r="D2" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E2" s="6">
+      <c r="D2" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E2" s="5">
         <v>0.0</v>
       </c>
-      <c r="F2" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G2" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="F2" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" ht="13.5" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -484,24 +470,24 @@
       <c r="C3" s="2">
         <v>3.2</v>
       </c>
-      <c r="D3" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E3" s="6">
+      <c r="D3" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E3" s="5">
         <v>0.0</v>
       </c>
-      <c r="F3" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G3" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="F3" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" ht="13.5" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -510,24 +496,24 @@
       <c r="C4" s="2">
         <v>1.1</v>
       </c>
-      <c r="D4" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E4" s="6">
+      <c r="D4" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E4" s="5">
         <v>0.0</v>
       </c>
-      <c r="F4" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G4" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="F4" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" ht="13.5" customHeight="1">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -536,24 +522,24 @@
       <c r="C5" s="2">
         <v>5.5</v>
       </c>
-      <c r="D5" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E5" s="6">
+      <c r="D5" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E5" s="5">
         <v>0.0</v>
       </c>
-      <c r="F5" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G5" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H5" s="3" t="s">
+      <c r="F5" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" ht="13.5" customHeight="1">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -562,24 +548,24 @@
       <c r="C6" s="2">
         <v>4.2</v>
       </c>
-      <c r="D6" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E6" s="6">
+      <c r="D6" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E6" s="5">
         <v>0.0</v>
       </c>
-      <c r="F6" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G6" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H6" s="3" t="s">
+      <c r="F6" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -588,24 +574,24 @@
       <c r="C7" s="2">
         <v>4.1</v>
       </c>
-      <c r="D7" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E7" s="6">
+      <c r="D7" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E7" s="5">
         <v>0.0</v>
       </c>
-      <c r="F7" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G7" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H7" s="3" t="s">
+      <c r="F7" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" ht="13.5" customHeight="1">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -614,24 +600,24 @@
       <c r="C8" s="2">
         <v>6.5</v>
       </c>
-      <c r="D8" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E8" s="6">
+      <c r="D8" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E8" s="5">
         <v>0.0</v>
       </c>
-      <c r="F8" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G8" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H8" s="3" t="s">
+      <c r="F8" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" ht="13.5" customHeight="1">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -640,24 +626,24 @@
       <c r="C9" s="2">
         <v>4.3</v>
       </c>
-      <c r="D9" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E9" s="6">
+      <c r="D9" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E9" s="5">
         <v>0.0</v>
       </c>
-      <c r="F9" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G9" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H9" s="3" t="s">
+      <c r="F9" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" ht="13.5" customHeight="1">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -666,259 +652,328 @@
       <c r="C10" s="2">
         <v>2.1</v>
       </c>
-      <c r="D10" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E10" s="6">
+      <c r="D10" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E10" s="5">
         <v>0.0</v>
       </c>
-      <c r="F10" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G10" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H10" s="3" t="s">
+      <c r="F10" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" ht="13.5" customHeight="1">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="2">
         <v>1.0</v>
       </c>
-      <c r="D11" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E11" s="6">
+      <c r="D11" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E11" s="5">
         <v>0.0</v>
       </c>
-      <c r="F11" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G11" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H11" s="3" t="s">
+      <c r="F11" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G11" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" ht="13.5" customHeight="1">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="2">
         <v>3.0</v>
       </c>
-      <c r="D12" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E12" s="6">
+      <c r="D12" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E12" s="5">
         <v>0.0</v>
       </c>
-      <c r="F12" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G12" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H12" s="3" t="s">
+      <c r="F12" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G12" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" ht="13.5" customHeight="1">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="2">
         <v>4.0</v>
       </c>
-      <c r="D13" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E13" s="6">
+      <c r="D13" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E13" s="5">
         <v>0.0</v>
       </c>
-      <c r="F13" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G13" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H13" s="3" t="s">
+      <c r="F13" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" ht="13.5" customHeight="1">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="2">
         <v>4.0</v>
       </c>
-      <c r="D14" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E14" s="6">
+      <c r="D14" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E14" s="5">
         <v>0.0</v>
       </c>
-      <c r="F14" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G14" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H14" s="3" t="s">
+      <c r="F14" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" ht="13.5" customHeight="1">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="2">
         <v>4.0</v>
       </c>
-      <c r="D15" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E15" s="6">
+      <c r="D15" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E15" s="5">
         <v>0.0</v>
       </c>
-      <c r="F15" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G15" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H15" s="3" t="s">
+      <c r="F15" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G15" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" ht="13.5" customHeight="1">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="2">
         <v>5.0</v>
       </c>
-      <c r="D16" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E16" s="6">
+      <c r="D16" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E16" s="5">
         <v>0.0</v>
       </c>
-      <c r="F16" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G16" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H16" s="3" t="s">
+      <c r="F16" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G16" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" ht="13.5" customHeight="1">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="2">
         <v>4.0</v>
       </c>
-      <c r="D17" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E17" s="6">
+      <c r="D17" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E17" s="5">
         <v>0.0</v>
       </c>
-      <c r="F17" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G17" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H17" s="3" t="s">
+      <c r="F17" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G17" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" ht="13.5" customHeight="1">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="2">
         <v>3.0</v>
       </c>
-      <c r="D18" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E18" s="6">
+      <c r="D18" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E18" s="5">
         <v>0.0</v>
       </c>
-      <c r="F18" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G18" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H18" s="3" t="s">
+      <c r="F18" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G18" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="19" ht="13.5" customHeight="1">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="2">
         <v>4.0</v>
       </c>
-      <c r="D19" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E19" s="6">
+      <c r="D19" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E19" s="5">
         <v>0.0</v>
       </c>
-      <c r="F19" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G19" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H19" s="3" t="s">
+      <c r="F19" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G19" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" ht="13.5" customHeight="1"/>
-    <row r="21" ht="13.5" customHeight="1"/>
-    <row r="22" ht="13.5" customHeight="1"/>
+    <row r="20" ht="13.5" customHeight="1">
+      <c r="A20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="F20" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G20" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" ht="13.5" customHeight="1">
+      <c r="A21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="F21" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G21" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" ht="13.5" customHeight="1">
+      <c r="A22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="F22" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G22" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="23" ht="13.5" customHeight="1"/>
     <row r="24" ht="13.5" customHeight="1"/>
     <row r="25" ht="13.5" customHeight="1"/>
@@ -1948,110 +2003,110 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>40179.0</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="2">
-        <f>COUNTIFS('Sheet 1'!D:D,B2,'Sheet 1'!A:A,A2,'Sheet 1'!B:B,C2)</f>
+        <f>COUNTIFS('Sheet 1'!D:D,B2,'Sheet 1'!A:A,A2,'Sheet 1'!B:B,C2,'Sheet 1'!C:C,"&lt;&gt;"&amp;"")</f>
         <v>3</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>40179.0</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="2">
-        <f>COUNTIFS('Sheet 1'!D:D,B3,'Sheet 1'!A:A,A3,'Sheet 1'!B:B,C3)</f>
+        <f>COUNTIFS('Sheet 1'!D:D,B3,'Sheet 1'!A:A,A3,'Sheet 1'!B:B,C3,'Sheet 1'!C:C,"&lt;&gt;"&amp;"")</f>
         <v>3</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>40179.0</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="2">
-        <f>COUNTIFS('Sheet 1'!D:D,B4,'Sheet 1'!A:A,A4,'Sheet 1'!B:B,C4)</f>
+        <f>COUNTIFS('Sheet 1'!D:D,B4,'Sheet 1'!A:A,A4,'Sheet 1'!B:B,C4,'Sheet 1'!C:C,"&lt;&gt;"&amp;"")</f>
         <v>3</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>40179.0</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="2">
-        <f>COUNTIFS('Sheet 1'!D:D,B5,'Sheet 1'!A:A,A5,'Sheet 1'!B:B,C5)</f>
+        <f>COUNTIFS('Sheet 1'!D:D,B5,'Sheet 1'!A:A,A5,'Sheet 1'!B:B,C5,'Sheet 1'!C:C,"&lt;&gt;"&amp;"")</f>
         <v>3</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>40179.0</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="2">
-        <f>COUNTIFS('Sheet 1'!D:D,B6,'Sheet 1'!A:A,A6,'Sheet 1'!B:B,C6)</f>
+        <f>COUNTIFS('Sheet 1'!D:D,B6,'Sheet 1'!A:A,A6,'Sheet 1'!B:B,C6,'Sheet 1'!C:C,"&lt;&gt;"&amp;"")</f>
         <v>3</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>40179.0</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="2">
-        <f>COUNTIFS('Sheet 1'!D:D,B7,'Sheet 1'!A:A,A7,'Sheet 1'!B:B,C7)</f>
+        <f>COUNTIFS('Sheet 1'!D:D,B7,'Sheet 1'!A:A,A7,'Sheet 1'!B:B,C7,'Sheet 1'!C:C,"&lt;&gt;"&amp;"")</f>
         <v>3</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="2">
         <v>2.0</v>
       </c>
     </row>
@@ -2093,10 +2148,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>40179.0</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -2106,15 +2161,15 @@
         <f>MINIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B2,'Sheet 1'!A:A,A2,'Sheet 1'!B:B,C2)</f>
         <v>1.1</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>40179.0</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -2124,15 +2179,15 @@
         <f>MINIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B3,'Sheet 1'!A:A,A3,'Sheet 1'!B:B,C3)</f>
         <v>4.1</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>40179.0</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -2142,15 +2197,15 @@
         <f>MINIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B4,'Sheet 1'!A:A,A4,'Sheet 1'!B:B,C4)</f>
         <v>2.1</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>40179.0</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -2160,15 +2215,15 @@
         <f>MINIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B5,'Sheet 1'!A:A,A5,'Sheet 1'!B:B,C5)</f>
         <v>1</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>40179.0</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -2178,15 +2233,15 @@
         <f>MINIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B6,'Sheet 1'!A:A,A6,'Sheet 1'!B:B,C6)</f>
         <v>4</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>40179.0</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -2196,7 +2251,7 @@
         <f>MINIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B7,'Sheet 1'!A:A,A7,'Sheet 1'!B:B,C7)</f>
         <v>3</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="2">
         <v>2.0</v>
       </c>
     </row>
@@ -2238,10 +2293,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>40179.0</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -2251,15 +2306,15 @@
         <f>MAXIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B2,'Sheet 1'!A:A,A2,'Sheet 1'!B:B,C2)</f>
         <v>4.5</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>40179.0</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -2269,15 +2324,15 @@
         <f>MAXIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B3,'Sheet 1'!A:A,A3,'Sheet 1'!B:B,C3)</f>
         <v>5.5</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>40179.0</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -2287,15 +2342,15 @@
         <f>MAXIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B4,'Sheet 1'!A:A,A4,'Sheet 1'!B:B,C4)</f>
         <v>6.5</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>40179.0</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -2305,15 +2360,15 @@
         <f>MAXIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B5,'Sheet 1'!A:A,A5,'Sheet 1'!B:B,C5)</f>
         <v>4</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>40179.0</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -2323,15 +2378,15 @@
         <f>MAXIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B6,'Sheet 1'!A:A,A6,'Sheet 1'!B:B,C6)</f>
         <v>5</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>40179.0</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -2341,7 +2396,7 @@
         <f>MAXIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B7,'Sheet 1'!A:A,A7,'Sheet 1'!B:B,C7)</f>
         <v>4</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="2">
         <v>2.0</v>
       </c>
     </row>
@@ -2383,28 +2438,28 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>40179.0</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="7">
         <f>AVERAGEIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B2,'Sheet 1'!A:A,A2,'Sheet 1'!B:B,C2)</f>
         <v>2.933333333</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>40179.0</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -2414,15 +2469,15 @@
         <f>AVERAGEIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B3,'Sheet 1'!A:A,A3,'Sheet 1'!B:B,C3)</f>
         <v>4.6</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>40179.0</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -2432,33 +2487,33 @@
         <f>AVERAGEIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B4,'Sheet 1'!A:A,A4,'Sheet 1'!B:B,C4)</f>
         <v>4.3</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>40179.0</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="7">
         <f>AVERAGEIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B5,'Sheet 1'!A:A,A5,'Sheet 1'!B:B,C5)</f>
         <v>2.666666667</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>40179.0</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -2468,15 +2523,15 @@
         <f>AVERAGEIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B6,'Sheet 1'!A:A,A6,'Sheet 1'!B:B,C6)</f>
         <v>4.333333333</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>40179.0</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -2486,7 +2541,7 @@
         <f>AVERAGEIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B7,'Sheet 1'!A:A,A7,'Sheet 1'!B:B,C7)</f>
         <v>3.666666667</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="2">
         <v>2.0</v>
       </c>
     </row>
@@ -2528,74 +2583,74 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>40179.0</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="2">
-        <f>COUNTIFS('Sheet 1'!D:D,B2,'Sheet 1'!B:B,C2,'Sheet 1'!H:H,"*"&amp;A2&amp;"*")</f>
-        <v>9</v>
-      </c>
-      <c r="E2" s="3">
+        <f>COUNTIFS('Sheet 1'!D:D,B2,'Sheet 1'!B:B,C2,'Sheet 1'!H:H,"*"&amp;A2&amp;"*",'Sheet 1'!C:C,"&lt;&gt;"&amp;"")</f>
+        <v>9</v>
+      </c>
+      <c r="E2" s="2">
         <v>1.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>40179.0</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="2">
-        <f>COUNTIFS('Sheet 1'!D:D,B3,'Sheet 1'!B:B,C3,'Sheet 1'!H:H,"*"&amp;A3&amp;"*")</f>
-        <v>9</v>
-      </c>
-      <c r="E3" s="3">
+        <f>COUNTIFS('Sheet 1'!D:D,B3,'Sheet 1'!B:B,C3,'Sheet 1'!H:H,"*"&amp;A3&amp;"*",'Sheet 1'!C:C,"&lt;&gt;"&amp;"")</f>
+        <v>9</v>
+      </c>
+      <c r="E3" s="2">
         <v>1.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>40179.0</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="2">
-        <f>COUNTIFS('Sheet 1'!D:D,B4,'Sheet 1'!B:B,C4,'Sheet 1'!H:H,"*"&amp;A4&amp;"*")</f>
+        <f>COUNTIFS('Sheet 1'!D:D,B4,'Sheet 1'!B:B,C4,'Sheet 1'!H:H,"*"&amp;A4&amp;"*",'Sheet 1'!C:C,"&lt;&gt;"&amp;"")</f>
         <v>18</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>0.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="8"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
     <row r="6">
-      <c r="A6" s="8"/>
-      <c r="B6" s="5"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="8"/>
-      <c r="B7" s="5"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
@@ -2637,10 +2692,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>40179.0</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -2650,15 +2705,15 @@
         <f>MINIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B2,'Sheet 1'!B:B,C2,'Sheet 1'!H:H,"*"&amp;A2&amp;"*")</f>
         <v>1.1</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>1.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>40179.0</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -2668,15 +2723,15 @@
         <f>MINIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B3,'Sheet 1'!B:B,C3,'Sheet 1'!H:H,"*"&amp;A3&amp;"*")</f>
         <v>1</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>1.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>40179.0</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -2686,25 +2741,25 @@
         <f>MINIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B4,'Sheet 1'!B:B,C4,'Sheet 1'!H:H,"*"&amp;A4&amp;"*")</f>
         <v>1</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>0.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="8"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
     <row r="6">
-      <c r="A6" s="8"/>
-      <c r="B6" s="5"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="8"/>
-      <c r="B7" s="5"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
@@ -2746,10 +2801,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>40179.0</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -2759,15 +2814,15 @@
         <f>MAXIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B2,'Sheet 1'!B:B,C2,'Sheet 1'!H:H,"*"&amp;A2&amp;"*")</f>
         <v>6.5</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>1.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>40179.0</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -2777,15 +2832,15 @@
         <f>MAXIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B3,'Sheet 1'!B:B,C3,'Sheet 1'!H:H,"*"&amp;A3&amp;"*")</f>
         <v>5</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>1.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>40179.0</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -2795,25 +2850,25 @@
         <f>MAXIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B4,'Sheet 1'!B:B,C4,'Sheet 1'!H:H,"*"&amp;A4&amp;"*")</f>
         <v>6.5</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>0.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="8"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
     <row r="6">
-      <c r="A6" s="8"/>
-      <c r="B6" s="5"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="8"/>
-      <c r="B7" s="5"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
@@ -2855,10 +2910,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>40179.0</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -2868,15 +2923,15 @@
         <f>AVERAGEIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B2,'Sheet 1'!B:B,C2,'Sheet 1'!H:H,"*"&amp;A2&amp;"*")</f>
         <v>3.944444444</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>1.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>40179.0</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -2886,15 +2941,15 @@
         <f>AVERAGEIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B3,'Sheet 1'!B:B,C3,'Sheet 1'!H:H,"*"&amp;A3&amp;"*")</f>
         <v>3.555555556</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>1.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>40179.0</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -2904,25 +2959,25 @@
         <f>AVERAGEIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B4,'Sheet 1'!B:B,C4,'Sheet 1'!H:H,"*"&amp;A4&amp;"*")</f>
         <v>3.75</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>0.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="8"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
     <row r="6">
-      <c r="A6" s="8"/>
-      <c r="B6" s="5"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="8"/>
-      <c r="B7" s="5"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>

</xml_diff>

<commit_message>
[Version 1.40.2] Bug fixing (#261)
* Fix checking record when key has dot on it

* Allow null value on importer

* Bump version 1.40.2

* Fix codes for tests

* Fix query of RT on importer
</commit_message>
<xml_diff>
--- a/django_project/geosight/importer/tests/importers/_fixtures/excel_long_indicator_value (Multiple Value).xlsx
+++ b/django_project/geosight/importer/tests/importers/_fixtures/excel_long_indicator_value (Multiple Value).xlsx
@@ -16,15 +16,15 @@
   <definedNames/>
   <calcPr/>
   <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataSignature="AMtx7mi+UXBatFQzSAx8cjkAiPuZUmlApg=="/>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataChecksum="bmnISD6dnFMPociqsA5vDh98py0/G5yI1GEptyUpKng="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="20">
   <si>
     <t>geom_code</t>
   </si>
@@ -96,7 +96,7 @@
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -111,11 +111,6 @@
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -137,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -146,9 +141,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
@@ -157,12 +149,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="167" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
@@ -444,12 +430,12 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" ht="13.5" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -458,24 +444,24 @@
       <c r="C2" s="2">
         <v>4.5</v>
       </c>
-      <c r="D2" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E2" s="6">
+      <c r="D2" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E2" s="5">
         <v>0.0</v>
       </c>
-      <c r="F2" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G2" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="F2" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" ht="13.5" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -484,24 +470,24 @@
       <c r="C3" s="2">
         <v>3.2</v>
       </c>
-      <c r="D3" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E3" s="6">
+      <c r="D3" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E3" s="5">
         <v>0.0</v>
       </c>
-      <c r="F3" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G3" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="F3" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" ht="13.5" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -510,24 +496,24 @@
       <c r="C4" s="2">
         <v>1.1</v>
       </c>
-      <c r="D4" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E4" s="6">
+      <c r="D4" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E4" s="5">
         <v>0.0</v>
       </c>
-      <c r="F4" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G4" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="F4" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" ht="13.5" customHeight="1">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -536,24 +522,24 @@
       <c r="C5" s="2">
         <v>5.5</v>
       </c>
-      <c r="D5" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E5" s="6">
+      <c r="D5" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E5" s="5">
         <v>0.0</v>
       </c>
-      <c r="F5" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G5" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H5" s="3" t="s">
+      <c r="F5" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" ht="13.5" customHeight="1">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -562,24 +548,24 @@
       <c r="C6" s="2">
         <v>4.2</v>
       </c>
-      <c r="D6" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E6" s="6">
+      <c r="D6" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E6" s="5">
         <v>0.0</v>
       </c>
-      <c r="F6" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G6" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H6" s="3" t="s">
+      <c r="F6" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -588,24 +574,24 @@
       <c r="C7" s="2">
         <v>4.1</v>
       </c>
-      <c r="D7" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E7" s="6">
+      <c r="D7" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E7" s="5">
         <v>0.0</v>
       </c>
-      <c r="F7" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G7" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H7" s="3" t="s">
+      <c r="F7" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" ht="13.5" customHeight="1">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -614,24 +600,24 @@
       <c r="C8" s="2">
         <v>6.5</v>
       </c>
-      <c r="D8" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E8" s="6">
+      <c r="D8" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E8" s="5">
         <v>0.0</v>
       </c>
-      <c r="F8" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G8" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H8" s="3" t="s">
+      <c r="F8" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" ht="13.5" customHeight="1">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -640,24 +626,24 @@
       <c r="C9" s="2">
         <v>4.3</v>
       </c>
-      <c r="D9" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E9" s="6">
+      <c r="D9" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E9" s="5">
         <v>0.0</v>
       </c>
-      <c r="F9" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G9" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H9" s="3" t="s">
+      <c r="F9" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" ht="13.5" customHeight="1">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -666,259 +652,328 @@
       <c r="C10" s="2">
         <v>2.1</v>
       </c>
-      <c r="D10" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E10" s="6">
+      <c r="D10" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E10" s="5">
         <v>0.0</v>
       </c>
-      <c r="F10" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G10" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H10" s="3" t="s">
+      <c r="F10" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" ht="13.5" customHeight="1">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="2">
         <v>1.0</v>
       </c>
-      <c r="D11" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E11" s="6">
+      <c r="D11" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E11" s="5">
         <v>0.0</v>
       </c>
-      <c r="F11" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G11" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H11" s="3" t="s">
+      <c r="F11" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G11" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" ht="13.5" customHeight="1">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="2">
         <v>3.0</v>
       </c>
-      <c r="D12" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E12" s="6">
+      <c r="D12" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E12" s="5">
         <v>0.0</v>
       </c>
-      <c r="F12" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G12" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H12" s="3" t="s">
+      <c r="F12" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G12" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" ht="13.5" customHeight="1">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="2">
         <v>4.0</v>
       </c>
-      <c r="D13" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E13" s="6">
+      <c r="D13" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E13" s="5">
         <v>0.0</v>
       </c>
-      <c r="F13" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G13" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H13" s="3" t="s">
+      <c r="F13" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" ht="13.5" customHeight="1">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="2">
         <v>4.0</v>
       </c>
-      <c r="D14" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E14" s="6">
+      <c r="D14" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E14" s="5">
         <v>0.0</v>
       </c>
-      <c r="F14" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G14" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H14" s="3" t="s">
+      <c r="F14" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" ht="13.5" customHeight="1">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="2">
         <v>4.0</v>
       </c>
-      <c r="D15" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E15" s="6">
+      <c r="D15" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E15" s="5">
         <v>0.0</v>
       </c>
-      <c r="F15" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G15" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H15" s="3" t="s">
+      <c r="F15" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G15" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" ht="13.5" customHeight="1">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="2">
         <v>5.0</v>
       </c>
-      <c r="D16" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E16" s="6">
+      <c r="D16" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E16" s="5">
         <v>0.0</v>
       </c>
-      <c r="F16" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G16" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H16" s="3" t="s">
+      <c r="F16" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G16" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" ht="13.5" customHeight="1">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="2">
         <v>4.0</v>
       </c>
-      <c r="D17" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E17" s="6">
+      <c r="D17" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E17" s="5">
         <v>0.0</v>
       </c>
-      <c r="F17" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G17" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H17" s="3" t="s">
+      <c r="F17" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G17" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" ht="13.5" customHeight="1">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="2">
         <v>3.0</v>
       </c>
-      <c r="D18" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E18" s="6">
+      <c r="D18" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E18" s="5">
         <v>0.0</v>
       </c>
-      <c r="F18" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G18" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H18" s="3" t="s">
+      <c r="F18" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G18" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="19" ht="13.5" customHeight="1">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="2">
         <v>4.0</v>
       </c>
-      <c r="D19" s="5">
-        <v>40179.0</v>
-      </c>
-      <c r="E19" s="6">
+      <c r="D19" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E19" s="5">
         <v>0.0</v>
       </c>
-      <c r="F19" s="7">
-        <v>40179.0</v>
-      </c>
-      <c r="G19" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="H19" s="3" t="s">
+      <c r="F19" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G19" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" ht="13.5" customHeight="1"/>
-    <row r="21" ht="13.5" customHeight="1"/>
-    <row r="22" ht="13.5" customHeight="1"/>
+    <row r="20" ht="13.5" customHeight="1">
+      <c r="A20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="F20" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G20" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" ht="13.5" customHeight="1">
+      <c r="A21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="F21" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G21" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" ht="13.5" customHeight="1">
+      <c r="A22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="4">
+        <v>40179.0</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="F22" s="6">
+        <v>40179.0</v>
+      </c>
+      <c r="G22" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="23" ht="13.5" customHeight="1"/>
     <row r="24" ht="13.5" customHeight="1"/>
     <row r="25" ht="13.5" customHeight="1"/>
@@ -1948,110 +2003,110 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>40179.0</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="2">
-        <f>COUNTIFS('Sheet 1'!D:D,B2,'Sheet 1'!A:A,A2,'Sheet 1'!B:B,C2)</f>
+        <f>COUNTIFS('Sheet 1'!D:D,B2,'Sheet 1'!A:A,A2,'Sheet 1'!B:B,C2,'Sheet 1'!C:C,"&lt;&gt;"&amp;"")</f>
         <v>3</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>40179.0</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="2">
-        <f>COUNTIFS('Sheet 1'!D:D,B3,'Sheet 1'!A:A,A3,'Sheet 1'!B:B,C3)</f>
+        <f>COUNTIFS('Sheet 1'!D:D,B3,'Sheet 1'!A:A,A3,'Sheet 1'!B:B,C3,'Sheet 1'!C:C,"&lt;&gt;"&amp;"")</f>
         <v>3</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>40179.0</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="2">
-        <f>COUNTIFS('Sheet 1'!D:D,B4,'Sheet 1'!A:A,A4,'Sheet 1'!B:B,C4)</f>
+        <f>COUNTIFS('Sheet 1'!D:D,B4,'Sheet 1'!A:A,A4,'Sheet 1'!B:B,C4,'Sheet 1'!C:C,"&lt;&gt;"&amp;"")</f>
         <v>3</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>40179.0</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="2">
-        <f>COUNTIFS('Sheet 1'!D:D,B5,'Sheet 1'!A:A,A5,'Sheet 1'!B:B,C5)</f>
+        <f>COUNTIFS('Sheet 1'!D:D,B5,'Sheet 1'!A:A,A5,'Sheet 1'!B:B,C5,'Sheet 1'!C:C,"&lt;&gt;"&amp;"")</f>
         <v>3</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>40179.0</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="2">
-        <f>COUNTIFS('Sheet 1'!D:D,B6,'Sheet 1'!A:A,A6,'Sheet 1'!B:B,C6)</f>
+        <f>COUNTIFS('Sheet 1'!D:D,B6,'Sheet 1'!A:A,A6,'Sheet 1'!B:B,C6,'Sheet 1'!C:C,"&lt;&gt;"&amp;"")</f>
         <v>3</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>40179.0</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="2">
-        <f>COUNTIFS('Sheet 1'!D:D,B7,'Sheet 1'!A:A,A7,'Sheet 1'!B:B,C7)</f>
+        <f>COUNTIFS('Sheet 1'!D:D,B7,'Sheet 1'!A:A,A7,'Sheet 1'!B:B,C7,'Sheet 1'!C:C,"&lt;&gt;"&amp;"")</f>
         <v>3</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="2">
         <v>2.0</v>
       </c>
     </row>
@@ -2093,10 +2148,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>40179.0</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -2106,15 +2161,15 @@
         <f>MINIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B2,'Sheet 1'!A:A,A2,'Sheet 1'!B:B,C2)</f>
         <v>1.1</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>40179.0</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -2124,15 +2179,15 @@
         <f>MINIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B3,'Sheet 1'!A:A,A3,'Sheet 1'!B:B,C3)</f>
         <v>4.1</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>40179.0</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -2142,15 +2197,15 @@
         <f>MINIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B4,'Sheet 1'!A:A,A4,'Sheet 1'!B:B,C4)</f>
         <v>2.1</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>40179.0</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -2160,15 +2215,15 @@
         <f>MINIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B5,'Sheet 1'!A:A,A5,'Sheet 1'!B:B,C5)</f>
         <v>1</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>40179.0</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -2178,15 +2233,15 @@
         <f>MINIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B6,'Sheet 1'!A:A,A6,'Sheet 1'!B:B,C6)</f>
         <v>4</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>40179.0</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -2196,7 +2251,7 @@
         <f>MINIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B7,'Sheet 1'!A:A,A7,'Sheet 1'!B:B,C7)</f>
         <v>3</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="2">
         <v>2.0</v>
       </c>
     </row>
@@ -2238,10 +2293,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>40179.0</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -2251,15 +2306,15 @@
         <f>MAXIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B2,'Sheet 1'!A:A,A2,'Sheet 1'!B:B,C2)</f>
         <v>4.5</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>40179.0</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -2269,15 +2324,15 @@
         <f>MAXIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B3,'Sheet 1'!A:A,A3,'Sheet 1'!B:B,C3)</f>
         <v>5.5</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>40179.0</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -2287,15 +2342,15 @@
         <f>MAXIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B4,'Sheet 1'!A:A,A4,'Sheet 1'!B:B,C4)</f>
         <v>6.5</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>40179.0</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -2305,15 +2360,15 @@
         <f>MAXIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B5,'Sheet 1'!A:A,A5,'Sheet 1'!B:B,C5)</f>
         <v>4</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>40179.0</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -2323,15 +2378,15 @@
         <f>MAXIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B6,'Sheet 1'!A:A,A6,'Sheet 1'!B:B,C6)</f>
         <v>5</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>40179.0</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -2341,7 +2396,7 @@
         <f>MAXIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B7,'Sheet 1'!A:A,A7,'Sheet 1'!B:B,C7)</f>
         <v>4</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="2">
         <v>2.0</v>
       </c>
     </row>
@@ -2383,28 +2438,28 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>40179.0</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="7">
         <f>AVERAGEIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B2,'Sheet 1'!A:A,A2,'Sheet 1'!B:B,C2)</f>
         <v>2.933333333</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>40179.0</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -2414,15 +2469,15 @@
         <f>AVERAGEIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B3,'Sheet 1'!A:A,A3,'Sheet 1'!B:B,C3)</f>
         <v>4.6</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>40179.0</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -2432,33 +2487,33 @@
         <f>AVERAGEIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B4,'Sheet 1'!A:A,A4,'Sheet 1'!B:B,C4)</f>
         <v>4.3</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>40179.0</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="7">
         <f>AVERAGEIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B5,'Sheet 1'!A:A,A5,'Sheet 1'!B:B,C5)</f>
         <v>2.666666667</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>40179.0</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -2468,15 +2523,15 @@
         <f>AVERAGEIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B6,'Sheet 1'!A:A,A6,'Sheet 1'!B:B,C6)</f>
         <v>4.333333333</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="2">
         <v>2.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>40179.0</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -2486,7 +2541,7 @@
         <f>AVERAGEIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B7,'Sheet 1'!A:A,A7,'Sheet 1'!B:B,C7)</f>
         <v>3.666666667</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="2">
         <v>2.0</v>
       </c>
     </row>
@@ -2528,74 +2583,74 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>40179.0</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="2">
-        <f>COUNTIFS('Sheet 1'!D:D,B2,'Sheet 1'!B:B,C2,'Sheet 1'!H:H,"*"&amp;A2&amp;"*")</f>
-        <v>9</v>
-      </c>
-      <c r="E2" s="3">
+        <f>COUNTIFS('Sheet 1'!D:D,B2,'Sheet 1'!B:B,C2,'Sheet 1'!H:H,"*"&amp;A2&amp;"*",'Sheet 1'!C:C,"&lt;&gt;"&amp;"")</f>
+        <v>9</v>
+      </c>
+      <c r="E2" s="2">
         <v>1.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>40179.0</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="2">
-        <f>COUNTIFS('Sheet 1'!D:D,B3,'Sheet 1'!B:B,C3,'Sheet 1'!H:H,"*"&amp;A3&amp;"*")</f>
-        <v>9</v>
-      </c>
-      <c r="E3" s="3">
+        <f>COUNTIFS('Sheet 1'!D:D,B3,'Sheet 1'!B:B,C3,'Sheet 1'!H:H,"*"&amp;A3&amp;"*",'Sheet 1'!C:C,"&lt;&gt;"&amp;"")</f>
+        <v>9</v>
+      </c>
+      <c r="E3" s="2">
         <v>1.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>40179.0</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="2">
-        <f>COUNTIFS('Sheet 1'!D:D,B4,'Sheet 1'!B:B,C4,'Sheet 1'!H:H,"*"&amp;A4&amp;"*")</f>
+        <f>COUNTIFS('Sheet 1'!D:D,B4,'Sheet 1'!B:B,C4,'Sheet 1'!H:H,"*"&amp;A4&amp;"*",'Sheet 1'!C:C,"&lt;&gt;"&amp;"")</f>
         <v>18</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>0.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="8"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
     <row r="6">
-      <c r="A6" s="8"/>
-      <c r="B6" s="5"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="8"/>
-      <c r="B7" s="5"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
@@ -2637,10 +2692,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>40179.0</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -2650,15 +2705,15 @@
         <f>MINIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B2,'Sheet 1'!B:B,C2,'Sheet 1'!H:H,"*"&amp;A2&amp;"*")</f>
         <v>1.1</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>1.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>40179.0</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -2668,15 +2723,15 @@
         <f>MINIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B3,'Sheet 1'!B:B,C3,'Sheet 1'!H:H,"*"&amp;A3&amp;"*")</f>
         <v>1</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>1.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>40179.0</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -2686,25 +2741,25 @@
         <f>MINIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B4,'Sheet 1'!B:B,C4,'Sheet 1'!H:H,"*"&amp;A4&amp;"*")</f>
         <v>1</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>0.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="8"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
     <row r="6">
-      <c r="A6" s="8"/>
-      <c r="B6" s="5"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="8"/>
-      <c r="B7" s="5"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
@@ -2746,10 +2801,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>40179.0</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -2759,15 +2814,15 @@
         <f>MAXIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B2,'Sheet 1'!B:B,C2,'Sheet 1'!H:H,"*"&amp;A2&amp;"*")</f>
         <v>6.5</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>1.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>40179.0</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -2777,15 +2832,15 @@
         <f>MAXIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B3,'Sheet 1'!B:B,C3,'Sheet 1'!H:H,"*"&amp;A3&amp;"*")</f>
         <v>5</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>1.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>40179.0</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -2795,25 +2850,25 @@
         <f>MAXIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B4,'Sheet 1'!B:B,C4,'Sheet 1'!H:H,"*"&amp;A4&amp;"*")</f>
         <v>6.5</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>0.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="8"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
     <row r="6">
-      <c r="A6" s="8"/>
-      <c r="B6" s="5"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="8"/>
-      <c r="B7" s="5"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
@@ -2855,10 +2910,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>40179.0</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -2868,15 +2923,15 @@
         <f>AVERAGEIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B2,'Sheet 1'!B:B,C2,'Sheet 1'!H:H,"*"&amp;A2&amp;"*")</f>
         <v>3.944444444</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>1.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>40179.0</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -2886,15 +2941,15 @@
         <f>AVERAGEIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B3,'Sheet 1'!B:B,C3,'Sheet 1'!H:H,"*"&amp;A3&amp;"*")</f>
         <v>3.555555556</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>1.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>40179.0</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -2904,25 +2959,25 @@
         <f>AVERAGEIFS('Sheet 1'!C:C,'Sheet 1'!D:D,B4,'Sheet 1'!B:B,C4,'Sheet 1'!H:H,"*"&amp;A4&amp;"*")</f>
         <v>3.75</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>0.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="8"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
     <row r="6">
-      <c r="A6" s="8"/>
-      <c r="B6" s="5"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="8"/>
-      <c r="B7" s="5"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>

</xml_diff>